<commit_message>
Fixed partnership balancing equation. Manual calibration of acts per year and partnerships was peformed to match observed HIV and HPV prevalence patterns.
</commit_message>
<xml_diff>
--- a/Config/HIVParameters.xlsx
+++ b/Config/HIVParameters.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Demographics" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Actual" sheetId="6" r:id="rId4"/>
     <sheet name="Sheet2" sheetId="4" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="215">
   <si>
     <t>Male</t>
   </si>
@@ -430,16 +430,10 @@
     <t>Weller et al</t>
   </si>
   <si>
-    <t>Lei et al</t>
-  </si>
-  <si>
     <t>Source</t>
   </si>
   <si>
     <t>* Wide CI</t>
-  </si>
-  <si>
-    <t>* Probable publication bias</t>
   </si>
   <si>
     <t>15-19</t>
@@ -1359,14 +1353,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1968,7 +1962,7 @@
   <sheetData>
     <row r="1" spans="1:42" ht="60.5" thickBot="1">
       <c r="A1" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -2386,7 +2380,7 @@
         <v>1.2</v>
       </c>
       <c r="AH5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:42" ht="16" thickBot="1">
@@ -2466,7 +2460,7 @@
         <v>67.2</v>
       </c>
       <c r="AN6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:42" ht="16" thickBot="1">
@@ -3078,10 +3072,10 @@
     </row>
     <row r="15" spans="1:42" ht="31.5" thickBot="1">
       <c r="A15" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="F15" s="22" t="s">
         <v>98</v>
-      </c>
-      <c r="F15" s="22" t="s">
-        <v>100</v>
       </c>
       <c r="O15" s="3" t="s">
         <v>13</v>
@@ -3110,15 +3104,15 @@
     </row>
     <row r="16" spans="1:42" ht="15.5">
       <c r="Y16" s="38" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="17" spans="12:25" ht="15.5">
       <c r="O17" s="38" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="R17" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="Y17" s="37"/>
     </row>
@@ -3150,7 +3144,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:BF43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
@@ -3206,16 +3200,16 @@
         <v>60</v>
       </c>
       <c r="I1" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>127</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>129</v>
       </c>
       <c r="M1" s="2" t="s">
         <v>69</v>
@@ -3255,21 +3249,21 @@
       <c r="AF1" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="AI1" s="88" t="s">
+      <c r="AI1" s="89" t="s">
         <v>50</v>
       </c>
-      <c r="AJ1" s="89"/>
-      <c r="AK1" s="88" t="s">
+      <c r="AJ1" s="90"/>
+      <c r="AK1" s="89" t="s">
         <v>51</v>
       </c>
-      <c r="AL1" s="89"/>
-      <c r="AP1" s="90" t="s">
-        <v>155</v>
-      </c>
-      <c r="AQ1" s="90"/>
-      <c r="AR1" s="90"/>
-      <c r="AS1" s="90"/>
-      <c r="AT1" s="90"/>
+      <c r="AL1" s="90"/>
+      <c r="AP1" s="88" t="s">
+        <v>153</v>
+      </c>
+      <c r="AQ1" s="88"/>
+      <c r="AR1" s="88"/>
+      <c r="AS1" s="88"/>
+      <c r="AT1" s="88"/>
       <c r="AZ1" s="17" t="s">
         <v>66</v>
       </c>
@@ -3295,7 +3289,7 @@
       </c>
       <c r="E2" s="27"/>
       <c r="G2" s="11" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="H2" s="21">
         <v>7</v>
@@ -3316,7 +3310,7 @@
         <v>0.04</v>
       </c>
       <c r="P2" s="19" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="Q2" s="59">
         <v>0.34</v>
@@ -3363,25 +3357,25 @@
         <v>54</v>
       </c>
       <c r="AO2" s="32" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="AP2" s="24" t="s">
         <v>60</v>
       </c>
       <c r="AQ2" s="24" t="s">
+        <v>157</v>
+      </c>
+      <c r="AR2" s="24" t="s">
+        <v>158</v>
+      </c>
+      <c r="AS2" s="24" t="s">
         <v>159</v>
       </c>
-      <c r="AR2" s="24" t="s">
+      <c r="AT2" s="24" t="s">
         <v>160</v>
       </c>
-      <c r="AS2" s="24" t="s">
-        <v>161</v>
-      </c>
-      <c r="AT2" s="24" t="s">
-        <v>162</v>
-      </c>
       <c r="AU2" s="32" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="AZ2" s="18" t="s">
         <v>19</v>
@@ -3422,7 +3416,7 @@
       </c>
       <c r="E3" s="27"/>
       <c r="P3" s="19" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="Q3" s="59">
         <v>0.29199999999999998</v>
@@ -3529,7 +3523,7 @@
       </c>
       <c r="E4" s="27"/>
       <c r="H4" s="32" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="I4" s="32" t="s">
         <v>77</v>
@@ -3538,7 +3532,7 @@
         <v>78</v>
       </c>
       <c r="P4" s="20" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="Q4" s="58">
         <v>7.0999999999999994E-2</v>
@@ -3574,7 +3568,7 @@
         <v>0.24299999999999999</v>
       </c>
       <c r="AN4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="AO4" s="62" t="s">
         <v>1</v>
@@ -3636,7 +3630,7 @@
       </c>
       <c r="E5" s="23"/>
       <c r="G5" s="32" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="H5" s="18">
         <v>5.9999999999999995E-4</v>
@@ -3678,7 +3672,7 @@
         <v>0.25</v>
       </c>
       <c r="AO5" s="32" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="AP5" s="18">
         <v>0.25</v>
@@ -3736,7 +3730,7 @@
         <v>0.3</v>
       </c>
       <c r="G6" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="Z6" s="3" t="s">
         <v>5</v>
@@ -3836,13 +3830,13 @@
         <v>0.26100000000000001</v>
       </c>
       <c r="AO7" s="61"/>
-      <c r="AP7" s="90" t="s">
-        <v>158</v>
-      </c>
-      <c r="AQ7" s="90"/>
-      <c r="AR7" s="90"/>
-      <c r="AS7" s="90"/>
-      <c r="AT7" s="90"/>
+      <c r="AP7" s="88" t="s">
+        <v>156</v>
+      </c>
+      <c r="AQ7" s="88"/>
+      <c r="AR7" s="88"/>
+      <c r="AS7" s="88"/>
+      <c r="AT7" s="88"/>
       <c r="AZ7" s="19" t="s">
         <v>6</v>
       </c>
@@ -3887,16 +3881,16 @@
         <v>60</v>
       </c>
       <c r="I8" s="29" t="s">
+        <v>124</v>
+      </c>
+      <c r="J8" s="29" t="s">
+        <v>125</v>
+      </c>
+      <c r="K8" s="29" t="s">
         <v>126</v>
       </c>
-      <c r="J8" s="29" t="s">
+      <c r="L8" s="29" t="s">
         <v>127</v>
-      </c>
-      <c r="K8" s="29" t="s">
-        <v>128</v>
-      </c>
-      <c r="L8" s="29" t="s">
-        <v>129</v>
       </c>
       <c r="M8" s="29" t="s">
         <v>69</v>
@@ -3932,25 +3926,25 @@
         <v>0.26100000000000001</v>
       </c>
       <c r="AO8" s="32" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="AP8" s="32" t="s">
         <v>60</v>
       </c>
       <c r="AQ8" s="32" t="s">
+        <v>161</v>
+      </c>
+      <c r="AR8" s="32" t="s">
+        <v>162</v>
+      </c>
+      <c r="AS8" s="32" t="s">
         <v>163</v>
       </c>
-      <c r="AR8" s="32" t="s">
+      <c r="AT8" s="32" t="s">
         <v>164</v>
       </c>
-      <c r="AS8" s="32" t="s">
-        <v>165</v>
-      </c>
-      <c r="AT8" s="32" t="s">
-        <v>166</v>
-      </c>
       <c r="AU8" s="32" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="AZ8" s="19" t="s">
         <v>7</v>
@@ -3990,7 +3984,7 @@
         <v>0.3</v>
       </c>
       <c r="G9" s="48" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="H9" s="46">
         <f t="shared" ref="H9:M9" si="2">$H$5*H2</f>
@@ -4277,7 +4271,7 @@
         <v>0.26300000000000001</v>
       </c>
       <c r="AO11" s="32" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="AP11" s="18">
         <v>0.25</v>
@@ -4402,7 +4396,7 @@
         <v>0.3</v>
       </c>
       <c r="G13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="Z13" s="3" t="s">
         <v>12</v>
@@ -4493,15 +4487,15 @@
         <v>0</v>
       </c>
       <c r="AN14" t="s">
-        <v>137</v>
-      </c>
-      <c r="AP14" s="90" t="s">
-        <v>191</v>
-      </c>
-      <c r="AQ14" s="90"/>
-      <c r="AR14" s="90"/>
-      <c r="AS14" s="90"/>
-      <c r="AT14" s="90"/>
+        <v>135</v>
+      </c>
+      <c r="AP14" s="88" t="s">
+        <v>189</v>
+      </c>
+      <c r="AQ14" s="88"/>
+      <c r="AR14" s="88"/>
+      <c r="AS14" s="88"/>
+      <c r="AT14" s="88"/>
       <c r="AZ14" s="19" t="s">
         <v>13</v>
       </c>
@@ -4526,7 +4520,7 @@
     </row>
     <row r="15" spans="1:58" ht="15.5">
       <c r="A15" s="74" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B15" s="76">
         <f t="shared" si="0"/>
@@ -4540,26 +4534,26 @@
         <v>0.3</v>
       </c>
       <c r="AO15" s="32" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="AP15" s="24" t="s">
         <v>60</v>
       </c>
       <c r="AQ15" s="24" t="s">
+        <v>157</v>
+      </c>
+      <c r="AR15" s="24" t="s">
+        <v>158</v>
+      </c>
+      <c r="AS15" s="24" t="s">
         <v>159</v>
       </c>
-      <c r="AR15" s="24" t="s">
+      <c r="AT15" s="24" t="s">
         <v>160</v>
-      </c>
-      <c r="AS15" s="24" t="s">
-        <v>161</v>
-      </c>
-      <c r="AT15" s="24" t="s">
-        <v>162</v>
       </c>
       <c r="AU15" s="53"/>
       <c r="AZ15" s="74" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="BA15" s="75">
         <v>0</v>
@@ -4582,7 +4576,7 @@
     </row>
     <row r="16" spans="1:58" ht="15.5">
       <c r="A16" s="74" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B16" s="76">
         <f t="shared" si="0"/>
@@ -4596,7 +4590,7 @@
         <v>0.3</v>
       </c>
       <c r="G16" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="AO16" s="32" t="s">
         <v>0</v>
@@ -4623,7 +4617,7 @@
       </c>
       <c r="AU16" s="23"/>
       <c r="AZ16" s="74" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="BA16" s="75">
         <v>0</v>
@@ -4646,7 +4640,7 @@
     </row>
     <row r="17" spans="1:58" ht="15.5">
       <c r="A17" s="74" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B17" s="76">
         <f t="shared" si="0"/>
@@ -4660,7 +4654,7 @@
         <v>0.3</v>
       </c>
       <c r="G17" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="AO17" s="62" t="s">
         <v>1</v>
@@ -4687,7 +4681,7 @@
       </c>
       <c r="AU17" s="23"/>
       <c r="AZ17" s="74" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="BA17" s="75">
         <v>0</v>
@@ -4710,7 +4704,7 @@
     </row>
     <row r="18" spans="1:58" ht="15.5">
       <c r="A18" s="74" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B18" s="76">
         <f t="shared" si="0"/>
@@ -4724,14 +4718,14 @@
         <v>0.3</v>
       </c>
       <c r="G18" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H18">
         <f>11/10^4</f>
         <v>1.1000000000000001E-3</v>
       </c>
       <c r="AO18" s="32" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="AP18" s="58">
         <f t="shared" si="6"/>
@@ -4755,7 +4749,7 @@
       </c>
       <c r="AU18" s="23"/>
       <c r="AZ18" s="74" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="BA18" s="75">
         <v>0</v>
@@ -4778,7 +4772,7 @@
     </row>
     <row r="19" spans="1:58">
       <c r="G19" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="H19">
         <f>138/10^4</f>
@@ -4788,41 +4782,41 @@
     </row>
     <row r="20" spans="1:58">
       <c r="AO20" s="61"/>
-      <c r="AP20" s="90" t="s">
-        <v>192</v>
-      </c>
-      <c r="AQ20" s="90"/>
-      <c r="AR20" s="90"/>
-      <c r="AS20" s="90"/>
-      <c r="AT20" s="90"/>
+      <c r="AP20" s="88" t="s">
+        <v>190</v>
+      </c>
+      <c r="AQ20" s="88"/>
+      <c r="AR20" s="88"/>
+      <c r="AS20" s="88"/>
+      <c r="AT20" s="88"/>
       <c r="AU20" s="23"/>
     </row>
     <row r="21" spans="1:58">
       <c r="G21" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="AO21" s="32" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="AP21" s="32" t="s">
         <v>60</v>
       </c>
       <c r="AQ21" s="32" t="s">
+        <v>161</v>
+      </c>
+      <c r="AR21" s="32" t="s">
+        <v>162</v>
+      </c>
+      <c r="AS21" s="32" t="s">
         <v>163</v>
       </c>
-      <c r="AR21" s="32" t="s">
+      <c r="AT21" s="32" t="s">
         <v>164</v>
-      </c>
-      <c r="AS21" s="32" t="s">
-        <v>165</v>
-      </c>
-      <c r="AT21" s="32" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="22" spans="1:58">
       <c r="G22" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="AO22" s="32" t="s">
         <v>0</v>
@@ -4851,7 +4845,7 @@
     </row>
     <row r="23" spans="1:58" ht="16" customHeight="1">
       <c r="G23" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H23">
         <f>4/10^4</f>
@@ -4884,14 +4878,14 @@
     </row>
     <row r="24" spans="1:58">
       <c r="G24" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="H24">
         <f>8/10^4</f>
         <v>8.0000000000000004E-4</v>
       </c>
       <c r="AO24" s="32" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="AP24" s="58">
         <f t="shared" si="9"/>
@@ -4917,7 +4911,7 @@
     </row>
     <row r="26" spans="1:58">
       <c r="G26" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="H26">
         <f>2260/10^4</f>
@@ -4926,75 +4920,75 @@
     </row>
     <row r="27" spans="1:58">
       <c r="A27" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B27">
         <f>COUNT(H2:M2,BA3:BF18,AP30:AS34,AP16:AS18,AP22:AS24,H23:H24,H26)</f>
         <v>149</v>
       </c>
       <c r="AO27" s="73" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="28" spans="1:58">
       <c r="G28" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="AO28" s="68"/>
-      <c r="AP28" s="90" t="s">
-        <v>209</v>
-      </c>
-      <c r="AQ28" s="90"/>
-      <c r="AR28" s="90"/>
-      <c r="AS28" s="90"/>
+      <c r="AP28" s="88" t="s">
+        <v>207</v>
+      </c>
+      <c r="AQ28" s="88"/>
+      <c r="AR28" s="88"/>
+      <c r="AS28" s="88"/>
       <c r="AT28" s="72"/>
       <c r="AU28" s="68"/>
-      <c r="AV28" s="90" t="s">
-        <v>208</v>
-      </c>
-      <c r="AW28" s="90"/>
-      <c r="AX28" s="90"/>
-      <c r="AY28" s="90"/>
+      <c r="AV28" s="88" t="s">
+        <v>206</v>
+      </c>
+      <c r="AW28" s="88"/>
+      <c r="AX28" s="88"/>
+      <c r="AY28" s="88"/>
     </row>
     <row r="29" spans="1:58" ht="30">
       <c r="G29" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="AO29" s="32" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="AP29" s="24" t="s">
         <v>60</v>
       </c>
       <c r="AQ29" s="24" t="s">
+        <v>157</v>
+      </c>
+      <c r="AR29" s="24" t="s">
+        <v>158</v>
+      </c>
+      <c r="AS29" s="24" t="s">
         <v>159</v>
-      </c>
-      <c r="AR29" s="24" t="s">
-        <v>160</v>
-      </c>
-      <c r="AS29" s="24" t="s">
-        <v>161</v>
       </c>
       <c r="AT29" s="71"/>
       <c r="AU29" s="32" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="AV29" s="24" t="s">
         <v>60</v>
       </c>
       <c r="AW29" s="24" t="s">
+        <v>157</v>
+      </c>
+      <c r="AX29" s="24" t="s">
+        <v>158</v>
+      </c>
+      <c r="AY29" s="24" t="s">
         <v>159</v>
-      </c>
-      <c r="AX29" s="24" t="s">
-        <v>160</v>
-      </c>
-      <c r="AY29" s="24" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="30" spans="1:58">
       <c r="G30" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="AO30" s="32" t="s">
         <v>60</v>
@@ -5036,7 +5030,7 @@
     </row>
     <row r="31" spans="1:58">
       <c r="AO31" s="62" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="AP31" s="58">
         <v>4</v>
@@ -5055,7 +5049,7 @@
       </c>
       <c r="AT31" s="52"/>
       <c r="AU31" s="62" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="AV31" s="58">
         <v>4</v>
@@ -5075,7 +5069,7 @@
     </row>
     <row r="32" spans="1:58">
       <c r="AO32" s="32" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="AP32" s="58">
         <f>4</f>
@@ -5095,7 +5089,7 @@
       </c>
       <c r="AT32" s="52"/>
       <c r="AU32" s="32" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="AV32" s="58">
         <f>4</f>
@@ -5116,7 +5110,7 @@
     </row>
     <row r="33" spans="41:51">
       <c r="AO33" s="32" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="AP33" s="58">
         <f>4</f>
@@ -5135,7 +5129,7 @@
         <v>0.10070493454179255</v>
       </c>
       <c r="AU33" s="32" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="AV33" s="58">
         <f>4</f>
@@ -5156,7 +5150,7 @@
     </row>
     <row r="34" spans="41:51">
       <c r="AO34" s="32" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="AP34" s="58">
         <v>4</v>
@@ -5174,7 +5168,7 @@
         <v>0.49261083743842371</v>
       </c>
       <c r="AU34" s="32" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="AV34" s="58">
         <v>4</v>
@@ -5194,56 +5188,56 @@
     </row>
     <row r="36" spans="41:51">
       <c r="AO36" s="73" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="37" spans="41:51" ht="31" customHeight="1">
       <c r="AO37" s="68"/>
-      <c r="AP37" s="90" t="s">
-        <v>206</v>
-      </c>
-      <c r="AQ37" s="90"/>
-      <c r="AR37" s="90"/>
-      <c r="AS37" s="90"/>
+      <c r="AP37" s="88" t="s">
+        <v>204</v>
+      </c>
+      <c r="AQ37" s="88"/>
+      <c r="AR37" s="88"/>
+      <c r="AS37" s="88"/>
       <c r="AU37" s="68"/>
-      <c r="AV37" s="90" t="s">
-        <v>207</v>
-      </c>
-      <c r="AW37" s="90"/>
-      <c r="AX37" s="90"/>
-      <c r="AY37" s="90"/>
+      <c r="AV37" s="88" t="s">
+        <v>205</v>
+      </c>
+      <c r="AW37" s="88"/>
+      <c r="AX37" s="88"/>
+      <c r="AY37" s="88"/>
     </row>
     <row r="38" spans="41:51">
       <c r="AO38" s="32" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="AP38" s="32" t="s">
         <v>60</v>
       </c>
       <c r="AQ38" s="62" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="AR38" s="32" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="AS38" s="32" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="AT38" s="53"/>
       <c r="AU38" s="32" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="AV38" s="32" t="s">
         <v>60</v>
       </c>
       <c r="AW38" s="62" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="AX38" s="32" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="AY38" s="32" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="39" spans="41:51" ht="30.5" customHeight="1">
@@ -5286,7 +5280,7 @@
     </row>
     <row r="40" spans="41:51" ht="15">
       <c r="AO40" s="24" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="AP40" s="58">
         <v>4</v>
@@ -5304,7 +5298,7 @@
         <v>0.2040816326530612</v>
       </c>
       <c r="AU40" s="24" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="AV40" s="58">
         <v>4</v>
@@ -5324,7 +5318,7 @@
     </row>
     <row r="41" spans="41:51" ht="15">
       <c r="AO41" s="24" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="AP41" s="58">
         <f>4</f>
@@ -5343,7 +5337,7 @@
         <v>0.45662100456621008</v>
       </c>
       <c r="AU41" s="24" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="AV41" s="58">
         <f>4</f>
@@ -5364,7 +5358,7 @@
     </row>
     <row r="42" spans="41:51" ht="15">
       <c r="AO42" s="24" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="AP42" s="58">
         <f>4</f>
@@ -5383,7 +5377,7 @@
         <v>0.47846889952153115</v>
       </c>
       <c r="AU42" s="24" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="AV42" s="58">
         <f>4</f>
@@ -5404,7 +5398,7 @@
     </row>
     <row r="43" spans="41:51">
       <c r="AO43" s="32" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="AP43" s="58">
         <v>4</v>
@@ -5422,7 +5416,7 @@
         <v>0.92592592592592582</v>
       </c>
       <c r="AU43" s="32" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="AV43" s="58">
         <v>4</v>
@@ -5442,16 +5436,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="AK1:AL1"/>
+    <mergeCell ref="AI1:AJ1"/>
+    <mergeCell ref="AP1:AT1"/>
+    <mergeCell ref="AP28:AS28"/>
+    <mergeCell ref="AV28:AY28"/>
     <mergeCell ref="AP37:AS37"/>
     <mergeCell ref="AV37:AY37"/>
     <mergeCell ref="AP7:AT7"/>
     <mergeCell ref="AP14:AT14"/>
     <mergeCell ref="AP20:AT20"/>
-    <mergeCell ref="AK1:AL1"/>
-    <mergeCell ref="AI1:AJ1"/>
-    <mergeCell ref="AP1:AT1"/>
-    <mergeCell ref="AP28:AS28"/>
-    <mergeCell ref="AV28:AY28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5464,8 +5458,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="B1:AF50"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Q3" sqref="Q3"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="R3" sqref="R3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -5487,24 +5481,24 @@
         <v>76</v>
       </c>
       <c r="AB1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="2:32">
       <c r="B2" s="32" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C2" s="32" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D2" s="32" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="E2" s="32" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F2" s="32" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="G2" s="32" t="s">
         <v>73</v>
@@ -5519,7 +5513,7 @@
         <v>78</v>
       </c>
       <c r="U2" s="18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="AB2" s="32" t="s">
         <v>70</v>
@@ -5536,7 +5530,7 @@
     </row>
     <row r="3" spans="2:32">
       <c r="B3" s="18" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C3" s="18">
         <v>2004</v>
@@ -5558,22 +5552,13 @@
         <v>75</v>
       </c>
       <c r="R3" s="58">
-        <v>0.7</v>
-      </c>
-      <c r="S3" s="18">
-        <v>0.62</v>
-      </c>
-      <c r="T3" s="18">
-        <v>0.76</v>
-      </c>
-      <c r="U3" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="V3" t="s">
-        <v>83</v>
-      </c>
+        <v>0.6</v>
+      </c>
+      <c r="S3" s="18"/>
+      <c r="T3" s="18"/>
+      <c r="U3" s="18"/>
       <c r="AB3" s="18" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="AC3" s="18">
         <v>0.02</v>
@@ -5585,12 +5570,12 @@
         <v>3.2000000000000001E-2</v>
       </c>
       <c r="AF3" s="36" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="2:32">
       <c r="B4" s="18" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C4" s="18">
         <v>2006</v>
@@ -5609,7 +5594,7 @@
         <v>0.12770640594149768</v>
       </c>
       <c r="Q4" s="18" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="R4" s="58">
         <v>0.8</v>
@@ -5624,10 +5609,10 @@
         <v>79</v>
       </c>
       <c r="V4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AB4" s="35" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="AC4" s="18">
         <v>9.0999999999999998E-2</v>
@@ -5649,7 +5634,7 @@
       <c r="F5" s="18"/>
       <c r="G5" s="18"/>
       <c r="AB5" s="35" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="AC5" s="18">
         <v>9.0999999999999998E-2</v>
@@ -5666,7 +5651,7 @@
       <c r="F6" s="23"/>
       <c r="G6" s="23"/>
       <c r="AB6" s="18" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="AC6" s="18">
         <v>33.299999999999997</v>
@@ -5678,7 +5663,7 @@
         <v>37.5</v>
       </c>
       <c r="AF6" s="36" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="7" spans="2:32">
@@ -5686,11 +5671,11 @@
       <c r="F7" s="23"/>
       <c r="G7" s="23"/>
       <c r="Q7" s="32" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="R7" s="18"/>
       <c r="AB7" s="18" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="AC7" s="18">
         <v>46.9</v>
@@ -5707,13 +5692,13 @@
       <c r="F8" s="23"/>
       <c r="G8" s="23"/>
       <c r="Q8" s="18" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="R8" s="18">
         <v>0.15</v>
       </c>
       <c r="AB8" s="18" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="AC8" s="18">
         <v>49.8</v>
@@ -5730,13 +5715,13 @@
       <c r="F9" s="23"/>
       <c r="G9" s="23"/>
       <c r="Q9" s="18" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="R9" s="18">
         <v>0.18</v>
       </c>
       <c r="AB9" s="18" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="AC9" s="18">
         <v>46.8</v>
@@ -5750,14 +5735,14 @@
     </row>
     <row r="10" spans="2:32">
       <c r="Q10" s="18" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="R10" s="58">
         <f>AVERAGE(R8:R9)</f>
         <v>0.16499999999999998</v>
       </c>
       <c r="AB10" s="32" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="AC10" s="33"/>
       <c r="AD10" s="34"/>
@@ -5765,7 +5750,7 @@
     </row>
     <row r="11" spans="2:32">
       <c r="AB11" s="18" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="AC11" s="18">
         <v>23.2</v>
@@ -5780,37 +5765,37 @@
     <row r="12" spans="2:32">
       <c r="X12" s="23"/>
       <c r="AB12" s="49" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="13" spans="2:32">
       <c r="Q13" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="14" spans="2:32">
       <c r="Q14" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="15" spans="2:32">
       <c r="AB15" s="32" t="s">
+        <v>136</v>
+      </c>
+      <c r="AC15" s="32" t="s">
+        <v>137</v>
+      </c>
+      <c r="AD15" s="32" t="s">
         <v>138</v>
-      </c>
-      <c r="AC15" s="32" t="s">
-        <v>139</v>
-      </c>
-      <c r="AD15" s="32" t="s">
-        <v>140</v>
       </c>
       <c r="AE15" s="53"/>
     </row>
     <row r="16" spans="2:32" ht="15.5">
       <c r="Q16" s="53" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="T16" s="53" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="AB16" s="18">
         <v>0</v>
@@ -5873,10 +5858,10 @@
     </row>
     <row r="19" spans="17:30" ht="15.5">
       <c r="Q19" s="36" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="T19" s="36" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="AB19" s="18">
         <v>3</v>
@@ -6291,19 +6276,19 @@
   <sheetData>
     <row r="1" spans="1:40" ht="41.5" customHeight="1">
       <c r="A1" s="31" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="I1" s="31" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="T1" s="31" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="AE1" s="39" t="s">
         <v>37</v>
       </c>
       <c r="AF1" s="40" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="AG1" s="41" t="s">
         <v>77</v>
@@ -6312,7 +6297,7 @@
         <v>78</v>
       </c>
       <c r="AI1" s="40" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="AJ1" s="41" t="s">
         <v>77</v>
@@ -6321,7 +6306,7 @@
         <v>78</v>
       </c>
       <c r="AL1" s="40" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="AM1" s="41" t="s">
         <v>77</v>
@@ -6332,24 +6317,24 @@
     </row>
     <row r="2" spans="1:40">
       <c r="A2" s="32" t="s">
+        <v>102</v>
+      </c>
+      <c r="B2" s="32" t="s">
+        <v>103</v>
+      </c>
+      <c r="C2" s="32" t="s">
         <v>104</v>
-      </c>
-      <c r="B2" s="32" t="s">
-        <v>105</v>
-      </c>
-      <c r="C2" s="32" t="s">
-        <v>106</v>
       </c>
       <c r="D2" s="32"/>
       <c r="E2" s="32" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F2" s="32"/>
       <c r="J2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="U2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="AE2" s="42">
         <v>2004</v>
@@ -6385,22 +6370,22 @@
     <row r="3" spans="1:40">
       <c r="B3" s="18"/>
       <c r="C3" s="18" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D3" s="18" t="s">
         <v>1</v>
       </c>
       <c r="E3" s="18" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F3" s="18" t="s">
         <v>1</v>
       </c>
       <c r="I3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="T3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="AE3" s="42">
         <v>2005</v>
@@ -6453,7 +6438,7 @@
         <v>0</v>
       </c>
       <c r="I4" s="18" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="J4" s="32">
         <v>2004</v>
@@ -6480,7 +6465,7 @@
         <v>2011</v>
       </c>
       <c r="T4" s="18" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="U4" s="32">
         <v>2004</v>
@@ -6557,7 +6542,7 @@
         <v>0</v>
       </c>
       <c r="I5" s="32" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="J5" s="45">
         <v>0.126</v>
@@ -6584,7 +6569,7 @@
         <v>0.14699999999999999</v>
       </c>
       <c r="T5" s="32" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="U5" s="45">
         <v>3.7999999999999999E-2</v>
@@ -6661,7 +6646,7 @@
         <v>0</v>
       </c>
       <c r="I6" s="32" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J6" s="45">
         <v>0.25600000000000001</v>
@@ -6688,7 +6673,7 @@
         <v>0.26500000000000001</v>
       </c>
       <c r="T6" s="32" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="U6" s="45">
         <v>8.3000000000000004E-2</v>
@@ -6765,7 +6750,7 @@
         <v>4.7E-2</v>
       </c>
       <c r="I7" s="32" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="J7" s="45">
         <v>0.38400000000000001</v>
@@ -6792,7 +6777,7 @@
         <v>0.38300000000000001</v>
       </c>
       <c r="T7" s="32" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="U7" s="45">
         <v>0.19600000000000001</v>
@@ -6869,7 +6854,7 @@
         <v>8.7999999999999995E-2</v>
       </c>
       <c r="I8" s="32" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="J8" s="45">
         <v>0.40899999999999997</v>
@@ -6896,7 +6881,7 @@
         <v>0.47099999999999997</v>
       </c>
       <c r="T8" s="32" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="U8" s="45">
         <v>0.30099999999999999</v>
@@ -6973,7 +6958,7 @@
         <v>0.125</v>
       </c>
       <c r="I9" s="32" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="J9" s="45">
         <v>0.35</v>
@@ -7000,7 +6985,7 @@
         <v>0.504</v>
       </c>
       <c r="T9" s="32" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="U9" s="45">
         <v>0.27100000000000002</v>
@@ -7077,7 +7062,7 @@
         <v>0.10299999999999999</v>
       </c>
       <c r="I10" s="32" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="J10" s="45">
         <v>0.3</v>
@@ -7104,7 +7089,7 @@
         <v>0.49099999999999999</v>
       </c>
       <c r="T10" s="32" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="U10" s="45">
         <v>0.27700000000000002</v>
@@ -7151,7 +7136,7 @@
         <v>9.1999999999999998E-2</v>
       </c>
       <c r="I11" s="32" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="J11" s="45">
         <v>0.29199999999999998</v>
@@ -7178,7 +7163,7 @@
         <v>0.503</v>
       </c>
       <c r="T11" s="32" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="U11" s="45">
         <v>0.22600000000000001</v>
@@ -7245,10 +7230,10 @@
         <v>6.7000000000000004E-2</v>
       </c>
       <c r="I13" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="T13" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="14" spans="1:40" ht="15.5">
@@ -7293,21 +7278,21 @@
     </row>
     <row r="16" spans="1:40">
       <c r="B16" t="s">
+        <v>107</v>
+      </c>
+      <c r="C16" t="s">
+        <v>108</v>
+      </c>
+      <c r="E16" t="s">
         <v>109</v>
-      </c>
-      <c r="C16" t="s">
-        <v>110</v>
-      </c>
-      <c r="E16" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="20" spans="1:24">
       <c r="A20" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E20" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="21" spans="1:24">
@@ -7344,16 +7329,16 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="I22" s="36" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="R22" s="67"/>
       <c r="S22" s="67" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="T22" s="67"/>
       <c r="U22" s="67"/>
       <c r="V22" s="67" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="W22" s="67"/>
       <c r="X22" s="67"/>
@@ -7379,22 +7364,22 @@
       </c>
       <c r="R23" s="67"/>
       <c r="S23" s="67" t="s">
+        <v>193</v>
+      </c>
+      <c r="T23" s="67" t="s">
+        <v>194</v>
+      </c>
+      <c r="U23" s="67" t="s">
         <v>195</v>
       </c>
-      <c r="T23" s="67" t="s">
-        <v>196</v>
-      </c>
-      <c r="U23" s="67" t="s">
-        <v>197</v>
-      </c>
       <c r="V23" s="67" t="s">
+        <v>193</v>
+      </c>
+      <c r="W23" s="67" t="s">
+        <v>194</v>
+      </c>
+      <c r="X23" s="67" t="s">
         <v>195</v>
-      </c>
-      <c r="W23" s="67" t="s">
-        <v>196</v>
-      </c>
-      <c r="X23" s="67" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="24" spans="1:24">
@@ -7540,7 +7525,7 @@
         <v>0.20250000000000001</v>
       </c>
       <c r="I27" s="36" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="R27" s="67">
         <v>2008</v>
@@ -7707,7 +7692,7 @@
         <v>0.192</v>
       </c>
       <c r="I31" s="36" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="R31" s="67">
         <v>2012</v>
@@ -7739,10 +7724,10 @@
         <v>0.16300000000000001</v>
       </c>
       <c r="C32" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E32" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F32" s="63"/>
       <c r="R32" s="67">
@@ -7847,7 +7832,7 @@
         <v>0.33600000000000002</v>
       </c>
       <c r="I36" s="36" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="37" spans="1:20">
@@ -7858,7 +7843,7 @@
         <v>0.26100000000000001</v>
       </c>
       <c r="R37" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="38" spans="1:20">
@@ -7870,10 +7855,10 @@
       </c>
       <c r="R38" s="68"/>
       <c r="S38" s="68" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="T38" s="68" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="39" spans="1:20">
@@ -7935,7 +7920,7 @@
         <v>0.26300000000000001</v>
       </c>
       <c r="C42" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="R42" s="68">
         <v>2007</v>
@@ -7955,7 +7940,7 @@
         <v>0.318</v>
       </c>
       <c r="C43" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="R43" s="68">
         <v>2008</v>

</xml_diff>

<commit_message>
Adding latest rough calibration changes. Edits pending for calibrator.
</commit_message>
<xml_diff>
--- a/Config/HIVParameters.xlsx
+++ b/Config/HIVParameters.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12450" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Demographics" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Actual" sheetId="6" r:id="rId4"/>
     <sheet name="Sheet2" sheetId="4" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="215">
   <si>
     <t>Male</t>
   </si>
@@ -983,7 +983,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -1144,11 +1144,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1320,6 +1331,7 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1970,35 +1982,35 @@
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="82" t="s">
+      <c r="F1" s="83" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="83" t="s">
-        <v>0</v>
-      </c>
-      <c r="H1" s="83"/>
-      <c r="I1" s="83"/>
-      <c r="J1" s="83" t="s">
+      <c r="G1" s="84" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" s="84"/>
+      <c r="I1" s="84"/>
+      <c r="J1" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="K1" s="83"/>
-      <c r="L1" s="83"/>
-      <c r="O1" s="84" t="s">
+      <c r="K1" s="84"/>
+      <c r="L1" s="84"/>
+      <c r="O1" s="85" t="s">
         <v>19</v>
       </c>
-      <c r="P1" s="80" t="s">
+      <c r="P1" s="81" t="s">
         <v>20</v>
       </c>
-      <c r="Q1" s="80" t="s">
+      <c r="Q1" s="81" t="s">
         <v>21</v>
       </c>
-      <c r="R1" s="77" t="s">
+      <c r="R1" s="78" t="s">
         <v>22</v>
       </c>
-      <c r="S1" s="78"/>
-      <c r="T1" s="78"/>
-      <c r="U1" s="78"/>
-      <c r="V1" s="79"/>
+      <c r="S1" s="79"/>
+      <c r="T1" s="79"/>
+      <c r="U1" s="79"/>
+      <c r="V1" s="80"/>
       <c r="Y1" s="5" t="s">
         <v>39</v>
       </c>
@@ -2044,7 +2056,7 @@
       <c r="C2" s="4">
         <v>417311</v>
       </c>
-      <c r="F2" s="82"/>
+      <c r="F2" s="83"/>
       <c r="G2" s="54" t="s">
         <v>15</v>
       </c>
@@ -2063,13 +2075,13 @@
       <c r="L2" s="54" t="s">
         <v>17</v>
       </c>
-      <c r="O2" s="85"/>
-      <c r="P2" s="87"/>
-      <c r="Q2" s="87"/>
-      <c r="R2" s="80" t="s">
+      <c r="O2" s="86"/>
+      <c r="P2" s="88"/>
+      <c r="Q2" s="88"/>
+      <c r="R2" s="81" t="s">
         <v>23</v>
       </c>
-      <c r="S2" s="80" t="s">
+      <c r="S2" s="81" t="s">
         <v>24</v>
       </c>
       <c r="T2" s="9" t="s">
@@ -2078,7 +2090,7 @@
       <c r="U2" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="V2" s="80" t="s">
+      <c r="V2" s="81" t="s">
         <v>29</v>
       </c>
       <c r="Y2" s="11"/>
@@ -2156,18 +2168,18 @@
       <c r="L3" s="19">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="O3" s="86"/>
-      <c r="P3" s="81"/>
-      <c r="Q3" s="81"/>
-      <c r="R3" s="81"/>
-      <c r="S3" s="81"/>
+      <c r="O3" s="87"/>
+      <c r="P3" s="82"/>
+      <c r="Q3" s="82"/>
+      <c r="R3" s="82"/>
+      <c r="S3" s="82"/>
       <c r="T3" s="7" t="s">
         <v>26</v>
       </c>
       <c r="U3" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="V3" s="81"/>
+      <c r="V3" s="82"/>
       <c r="Y3" s="3" t="s">
         <v>2</v>
       </c>
@@ -3142,10 +3154,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:BF43"/>
+  <dimension ref="A1:BG43"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="AV1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AZ11" sqref="AZ11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -3187,7 +3199,7 @@
     <col min="58" max="58" width="15.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:58" ht="61" customHeight="1" thickBot="1">
+    <row r="1" spans="1:59" ht="61" customHeight="1" thickBot="1">
       <c r="A1" s="25" t="s">
         <v>67</v>
       </c>
@@ -3249,21 +3261,21 @@
       <c r="AF1" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="AI1" s="89" t="s">
+      <c r="AI1" s="90" t="s">
         <v>50</v>
       </c>
-      <c r="AJ1" s="90"/>
-      <c r="AK1" s="89" t="s">
+      <c r="AJ1" s="91"/>
+      <c r="AK1" s="90" t="s">
         <v>51</v>
       </c>
-      <c r="AL1" s="90"/>
-      <c r="AP1" s="88" t="s">
+      <c r="AL1" s="91"/>
+      <c r="AP1" s="89" t="s">
         <v>153</v>
       </c>
-      <c r="AQ1" s="88"/>
-      <c r="AR1" s="88"/>
-      <c r="AS1" s="88"/>
-      <c r="AT1" s="88"/>
+      <c r="AQ1" s="89"/>
+      <c r="AR1" s="89"/>
+      <c r="AS1" s="89"/>
+      <c r="AT1" s="89"/>
       <c r="AZ1" s="17" t="s">
         <v>66</v>
       </c>
@@ -3274,7 +3286,7 @@
       <c r="BE1" s="18"/>
       <c r="BF1" s="18"/>
     </row>
-    <row r="2" spans="1:58" ht="62.5" thickBot="1">
+    <row r="2" spans="1:59" ht="62.5" thickBot="1">
       <c r="A2" s="28" t="s">
         <v>70</v>
       </c>
@@ -3398,8 +3410,11 @@
       <c r="BF2" s="18" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="3" spans="1:58" ht="47" thickBot="1">
+      <c r="BG2" s="77" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:59" ht="47" thickBot="1">
       <c r="A3" s="19" t="s">
         <v>2</v>
       </c>
@@ -3505,8 +3520,12 @@
       <c r="BF3" s="58">
         <v>0.47</v>
       </c>
-    </row>
-    <row r="4" spans="1:58" ht="62.5" thickBot="1">
+      <c r="BG3">
+        <f>0.15*BC3</f>
+        <v>7.0499999999999993E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:59" ht="62.5" thickBot="1">
       <c r="A4" s="19" t="s">
         <v>3</v>
       </c>
@@ -3601,7 +3620,8 @@
         <v>0.01</v>
       </c>
       <c r="BC4" s="59">
-        <v>0.01</v>
+        <f>0.5*BD4</f>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="BD4" s="59">
         <v>0.05</v>
@@ -3612,8 +3632,12 @@
       <c r="BF4" s="59">
         <v>0.27</v>
       </c>
-    </row>
-    <row r="5" spans="1:58" ht="16" thickBot="1">
+      <c r="BG4" s="68">
+        <f t="shared" ref="BG4:BG18" si="2">0.15*BC4</f>
+        <v>3.7499999999999999E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:59" ht="16" thickBot="1">
       <c r="A5" s="19" t="s">
         <v>4</v>
       </c>
@@ -3702,7 +3726,8 @@
         <v>0.01</v>
       </c>
       <c r="BC5" s="59">
-        <v>0.01</v>
+        <f t="shared" ref="BC5:BC18" si="3">0.5*BD5</f>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="BD5" s="59">
         <v>0.05</v>
@@ -3713,8 +3738,12 @@
       <c r="BF5" s="59">
         <v>0.27</v>
       </c>
-    </row>
-    <row r="6" spans="1:58" ht="16" thickBot="1">
+      <c r="BG5" s="68">
+        <f t="shared" si="2"/>
+        <v>3.7499999999999999E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:59" ht="16" thickBot="1">
       <c r="A6" s="19" t="s">
         <v>5</v>
       </c>
@@ -3772,7 +3801,8 @@
         <v>0.01</v>
       </c>
       <c r="BC6" s="59">
-        <v>0.01</v>
+        <f t="shared" si="3"/>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="BD6" s="59">
         <v>0.05</v>
@@ -3783,8 +3813,12 @@
       <c r="BF6" s="59">
         <v>0.27</v>
       </c>
-    </row>
-    <row r="7" spans="1:58" ht="16" thickBot="1">
+      <c r="BG6" s="68">
+        <f t="shared" si="2"/>
+        <v>3.7499999999999999E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:59" ht="16" thickBot="1">
       <c r="A7" s="19" t="s">
         <v>6</v>
       </c>
@@ -3830,13 +3864,13 @@
         <v>0.26100000000000001</v>
       </c>
       <c r="AO7" s="61"/>
-      <c r="AP7" s="88" t="s">
+      <c r="AP7" s="89" t="s">
         <v>156</v>
       </c>
-      <c r="AQ7" s="88"/>
-      <c r="AR7" s="88"/>
-      <c r="AS7" s="88"/>
-      <c r="AT7" s="88"/>
+      <c r="AQ7" s="89"/>
+      <c r="AR7" s="89"/>
+      <c r="AS7" s="89"/>
+      <c r="AT7" s="89"/>
       <c r="AZ7" s="19" t="s">
         <v>6</v>
       </c>
@@ -3847,7 +3881,8 @@
         <v>0.01</v>
       </c>
       <c r="BC7" s="59">
-        <v>0.01</v>
+        <f t="shared" si="3"/>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="BD7" s="59">
         <v>0.05</v>
@@ -3858,8 +3893,12 @@
       <c r="BF7" s="59">
         <v>0.27</v>
       </c>
-    </row>
-    <row r="8" spans="1:58" ht="45.5" thickBot="1">
+      <c r="BG7" s="68">
+        <f t="shared" si="2"/>
+        <v>3.7499999999999999E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:59" ht="45.5" thickBot="1">
       <c r="A8" s="19" t="s">
         <v>7</v>
       </c>
@@ -3956,7 +3995,8 @@
         <v>0.01</v>
       </c>
       <c r="BC8" s="59">
-        <v>0.01</v>
+        <f t="shared" si="3"/>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="BD8" s="59">
         <v>0.05</v>
@@ -3967,8 +4007,12 @@
       <c r="BF8" s="59">
         <v>0.27</v>
       </c>
-    </row>
-    <row r="9" spans="1:58" ht="16" thickBot="1">
+      <c r="BG8" s="68">
+        <f t="shared" si="2"/>
+        <v>3.7499999999999999E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:59" ht="16" thickBot="1">
       <c r="A9" s="19" t="s">
         <v>18</v>
       </c>
@@ -3987,27 +4031,27 @@
         <v>131</v>
       </c>
       <c r="H9" s="46">
-        <f t="shared" ref="H9:M9" si="2">$H$5*H2</f>
+        <f t="shared" ref="H9:M9" si="4">$H$5*H2</f>
         <v>4.1999999999999997E-3</v>
       </c>
       <c r="I9" s="46">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>5.9999999999999995E-4</v>
       </c>
       <c r="J9" s="46">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3.4799999999999996E-3</v>
       </c>
       <c r="K9" s="46">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4.1399999999999996E-3</v>
       </c>
       <c r="L9" s="46">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>7.1399999999999996E-3</v>
       </c>
       <c r="M9" s="46">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2.3999999999999997E-5</v>
       </c>
       <c r="Z9" s="3" t="s">
@@ -4071,7 +4115,8 @@
         <v>0.01</v>
       </c>
       <c r="BC9" s="59">
-        <v>0.01</v>
+        <f t="shared" si="3"/>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="BD9" s="59">
         <v>0.05</v>
@@ -4082,8 +4127,12 @@
       <c r="BF9" s="59">
         <v>0.27</v>
       </c>
-    </row>
-    <row r="10" spans="1:58" ht="16" thickBot="1">
+      <c r="BG9" s="68">
+        <f t="shared" si="2"/>
+        <v>3.7499999999999999E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:59" ht="16" thickBot="1">
       <c r="A10" s="19" t="s">
         <v>9</v>
       </c>
@@ -4102,27 +4151,27 @@
         <v>77</v>
       </c>
       <c r="H10" s="47">
-        <f t="shared" ref="H10:M10" si="3">$I$5*H2</f>
+        <f t="shared" ref="H10:M10" si="5">$I$5*H2</f>
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="I10" s="47">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.01</v>
       </c>
       <c r="J10" s="47">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>5.7999999999999996E-2</v>
       </c>
       <c r="K10" s="47">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>6.9000000000000006E-2</v>
       </c>
       <c r="L10" s="47">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.11900000000000001</v>
       </c>
       <c r="M10" s="47">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>4.0000000000000002E-4</v>
       </c>
       <c r="Z10" s="3" t="s">
@@ -4186,7 +4235,8 @@
         <v>0.01</v>
       </c>
       <c r="BC10" s="59">
-        <v>0.01</v>
+        <f t="shared" si="3"/>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="BD10" s="59">
         <v>0.05</v>
@@ -4197,8 +4247,12 @@
       <c r="BF10" s="59">
         <v>0.27</v>
       </c>
-    </row>
-    <row r="11" spans="1:58" ht="16" thickBot="1">
+      <c r="BG10" s="68">
+        <f t="shared" si="2"/>
+        <v>3.7499999999999999E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:59" ht="16" thickBot="1">
       <c r="A11" s="19" t="s">
         <v>10</v>
       </c>
@@ -4217,27 +4271,27 @@
         <v>78</v>
       </c>
       <c r="H11" s="47">
-        <f t="shared" ref="H11:M11" si="4">MIN($J$5*H2,1)</f>
+        <f t="shared" ref="H11:M11" si="6">MIN($J$5*H2,1)</f>
         <v>0.98000000000000009</v>
       </c>
       <c r="I11" s="47">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.14000000000000001</v>
       </c>
       <c r="J11" s="47">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.81200000000000006</v>
       </c>
       <c r="K11" s="47">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.96600000000000019</v>
       </c>
       <c r="L11" s="47">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="M11" s="47">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>5.6000000000000008E-3</v>
       </c>
       <c r="Z11" s="3" t="s">
@@ -4301,7 +4355,8 @@
         <v>0.01</v>
       </c>
       <c r="BC11" s="59">
-        <v>0.01</v>
+        <f t="shared" si="3"/>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="BD11" s="59">
         <v>0.05</v>
@@ -4312,8 +4367,12 @@
       <c r="BF11" s="59">
         <v>0.27</v>
       </c>
-    </row>
-    <row r="12" spans="1:58" ht="16" thickBot="1">
+      <c r="BG11" s="68">
+        <f t="shared" si="2"/>
+        <v>3.7499999999999999E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:59" ht="16" thickBot="1">
       <c r="A12" s="19" t="s">
         <v>11</v>
       </c>
@@ -4368,7 +4427,8 @@
         <v>0.01</v>
       </c>
       <c r="BC12" s="59">
-        <v>0.01</v>
+        <f t="shared" si="3"/>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="BD12" s="59">
         <v>0.05</v>
@@ -4379,8 +4439,12 @@
       <c r="BF12" s="59">
         <v>0.27</v>
       </c>
-    </row>
-    <row r="13" spans="1:58" ht="16" thickBot="1">
+      <c r="BG12" s="68">
+        <f t="shared" si="2"/>
+        <v>3.7499999999999999E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:59" ht="16" thickBot="1">
       <c r="A13" s="19" t="s">
         <v>12</v>
       </c>
@@ -4441,7 +4505,8 @@
         <v>0.01</v>
       </c>
       <c r="BC13" s="59">
-        <v>0.01</v>
+        <f t="shared" si="3"/>
+        <v>0.05</v>
       </c>
       <c r="BD13" s="59">
         <v>0.1</v>
@@ -4452,8 +4517,12 @@
       <c r="BF13" s="59">
         <v>0.54</v>
       </c>
-    </row>
-    <row r="14" spans="1:58" ht="16" thickBot="1">
+      <c r="BG13" s="68">
+        <f t="shared" si="2"/>
+        <v>7.4999999999999997E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:59" ht="16" thickBot="1">
       <c r="A14" s="19" t="s">
         <v>13</v>
       </c>
@@ -4489,13 +4558,13 @@
       <c r="AN14" t="s">
         <v>135</v>
       </c>
-      <c r="AP14" s="88" t="s">
+      <c r="AP14" s="89" t="s">
         <v>189</v>
       </c>
-      <c r="AQ14" s="88"/>
-      <c r="AR14" s="88"/>
-      <c r="AS14" s="88"/>
-      <c r="AT14" s="88"/>
+      <c r="AQ14" s="89"/>
+      <c r="AR14" s="89"/>
+      <c r="AS14" s="89"/>
+      <c r="AT14" s="89"/>
       <c r="AZ14" s="19" t="s">
         <v>13</v>
       </c>
@@ -4506,7 +4575,8 @@
         <v>0.02</v>
       </c>
       <c r="BC14" s="59">
-        <v>0.02</v>
+        <f t="shared" si="3"/>
+        <v>0.05</v>
       </c>
       <c r="BD14" s="59">
         <v>0.1</v>
@@ -4517,8 +4587,12 @@
       <c r="BF14" s="59">
         <v>0.54</v>
       </c>
-    </row>
-    <row r="15" spans="1:58" ht="15.5">
+      <c r="BG14" s="68">
+        <f t="shared" si="2"/>
+        <v>7.4999999999999997E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:59" ht="15.5">
       <c r="A15" s="74" t="s">
         <v>210</v>
       </c>
@@ -4561,8 +4635,9 @@
       <c r="BB15" s="75">
         <v>0.02</v>
       </c>
-      <c r="BC15" s="76">
-        <v>0.02</v>
+      <c r="BC15" s="59">
+        <f t="shared" si="3"/>
+        <v>0.05</v>
       </c>
       <c r="BD15" s="76">
         <v>0.1</v>
@@ -4573,8 +4648,12 @@
       <c r="BF15" s="76">
         <v>0.54</v>
       </c>
-    </row>
-    <row r="16" spans="1:58" ht="15.5">
+      <c r="BG15" s="68">
+        <f t="shared" si="2"/>
+        <v>7.4999999999999997E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:59" ht="15.5">
       <c r="A16" s="74" t="s">
         <v>211</v>
       </c>
@@ -4604,15 +4683,15 @@
         <v>0.58479532163742687</v>
       </c>
       <c r="AR16" s="58">
-        <f t="shared" ref="AR16:AT16" si="5">1/AR3</f>
+        <f t="shared" ref="AR16:AT16" si="7">1/AR3</f>
         <v>0.95238095238095233</v>
       </c>
       <c r="AS16" s="58">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.21231422505307856</v>
       </c>
       <c r="AT16" s="30">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.51020408163265307</v>
       </c>
       <c r="AU16" s="23"/>
@@ -4625,8 +4704,9 @@
       <c r="BB16" s="75">
         <v>0.02</v>
       </c>
-      <c r="BC16" s="76">
-        <v>0.02</v>
+      <c r="BC16" s="59">
+        <f t="shared" si="3"/>
+        <v>0.05</v>
       </c>
       <c r="BD16" s="76">
         <v>0.1</v>
@@ -4637,8 +4717,12 @@
       <c r="BF16" s="76">
         <v>0.54</v>
       </c>
-    </row>
-    <row r="17" spans="1:58" ht="15.5">
+      <c r="BG16" s="68">
+        <f t="shared" si="2"/>
+        <v>7.4999999999999997E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:59" ht="15.5">
       <c r="A17" s="74" t="s">
         <v>212</v>
       </c>
@@ -4660,23 +4744,23 @@
         <v>1</v>
       </c>
       <c r="AP17" s="58">
-        <f t="shared" ref="AP17:AP18" si="6">1/AP4</f>
+        <f t="shared" ref="AP17:AP18" si="8">1/AP4</f>
         <v>4</v>
       </c>
       <c r="AQ17" s="58">
-        <f t="shared" ref="AQ17:AT18" si="7">1/AQ4</f>
+        <f t="shared" ref="AQ17:AT18" si="9">1/AQ4</f>
         <v>0.51546391752577325</v>
       </c>
       <c r="AR17" s="58">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.7407407407407407</v>
       </c>
       <c r="AS17" s="58">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.14903129657228018</v>
       </c>
       <c r="AT17" s="30">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.51020408163265307</v>
       </c>
       <c r="AU17" s="23"/>
@@ -4689,8 +4773,9 @@
       <c r="BB17" s="75">
         <v>0.02</v>
       </c>
-      <c r="BC17" s="76">
-        <v>0.02</v>
+      <c r="BC17" s="59">
+        <f t="shared" si="3"/>
+        <v>0.05</v>
       </c>
       <c r="BD17" s="76">
         <v>0.1</v>
@@ -4701,8 +4786,12 @@
       <c r="BF17" s="76">
         <v>0.54</v>
       </c>
-    </row>
-    <row r="18" spans="1:58" ht="15.5">
+      <c r="BG17" s="68">
+        <f t="shared" si="2"/>
+        <v>7.4999999999999997E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:59" ht="15.5">
       <c r="A18" s="74" t="s">
         <v>213</v>
       </c>
@@ -4728,23 +4817,23 @@
         <v>155</v>
       </c>
       <c r="AP18" s="58">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>4</v>
       </c>
       <c r="AQ18" s="58">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.53191489361702127</v>
       </c>
       <c r="AR18" s="58">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.81967213114754101</v>
       </c>
       <c r="AS18" s="58">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.16949152542372881</v>
       </c>
       <c r="AT18" s="30">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.51020408163265307</v>
       </c>
       <c r="AU18" s="23"/>
@@ -4757,8 +4846,9 @@
       <c r="BB18" s="75">
         <v>0.02</v>
       </c>
-      <c r="BC18" s="76">
-        <v>0.02</v>
+      <c r="BC18" s="59">
+        <f t="shared" si="3"/>
+        <v>0.05</v>
       </c>
       <c r="BD18" s="76">
         <v>0.1</v>
@@ -4769,8 +4859,12 @@
       <c r="BF18" s="76">
         <v>0.54</v>
       </c>
-    </row>
-    <row r="19" spans="1:58">
+      <c r="BG18" s="68">
+        <f t="shared" si="2"/>
+        <v>7.4999999999999997E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:59">
       <c r="G19" t="s">
         <v>168</v>
       </c>
@@ -4780,18 +4874,18 @@
       </c>
       <c r="AU19" s="23"/>
     </row>
-    <row r="20" spans="1:58">
+    <row r="20" spans="1:59">
       <c r="AO20" s="61"/>
-      <c r="AP20" s="88" t="s">
+      <c r="AP20" s="89" t="s">
         <v>190</v>
       </c>
-      <c r="AQ20" s="88"/>
-      <c r="AR20" s="88"/>
-      <c r="AS20" s="88"/>
-      <c r="AT20" s="88"/>
+      <c r="AQ20" s="89"/>
+      <c r="AR20" s="89"/>
+      <c r="AS20" s="89"/>
+      <c r="AT20" s="89"/>
       <c r="AU20" s="23"/>
     </row>
-    <row r="21" spans="1:58">
+    <row r="21" spans="1:59">
       <c r="G21" t="s">
         <v>169</v>
       </c>
@@ -4814,7 +4908,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="22" spans="1:58">
+    <row r="22" spans="1:59">
       <c r="G22" t="s">
         <v>152</v>
       </c>
@@ -4830,20 +4924,20 @@
         <v>0.29069767441860467</v>
       </c>
       <c r="AR22" s="58">
-        <f t="shared" ref="AR22:AT22" si="8">1/AR9</f>
+        <f t="shared" ref="AR22:AT22" si="10">1/AR9</f>
         <v>0.68965517241379315</v>
       </c>
       <c r="AS22" s="58">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0.32894736842105265</v>
       </c>
       <c r="AT22" s="30">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="AU22" s="23"/>
     </row>
-    <row r="23" spans="1:58" ht="16" customHeight="1">
+    <row r="23" spans="1:59" ht="16" customHeight="1">
       <c r="G23" t="s">
         <v>167</v>
       </c>
@@ -4855,28 +4949,28 @@
         <v>1</v>
       </c>
       <c r="AP23" s="58">
-        <f t="shared" ref="AP23:AP24" si="9">1/AP10</f>
+        <f t="shared" ref="AP23:AP24" si="11">1/AP10</f>
         <v>4</v>
       </c>
       <c r="AQ23" s="58">
-        <f t="shared" ref="AQ23:AT24" si="10">1/AQ10</f>
+        <f t="shared" ref="AQ23:AT24" si="12">1/AQ10</f>
         <v>0.32679738562091504</v>
       </c>
       <c r="AR23" s="58">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0.44052863436123346</v>
       </c>
       <c r="AS23" s="58">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0.18348623853211007</v>
       </c>
       <c r="AT23" s="30">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0.84745762711864414</v>
       </c>
       <c r="AU23" s="23"/>
     </row>
-    <row r="24" spans="1:58">
+    <row r="24" spans="1:59">
       <c r="G24" t="s">
         <v>168</v>
       </c>
@@ -4888,28 +4982,28 @@
         <v>155</v>
       </c>
       <c r="AP24" s="58">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>4</v>
       </c>
       <c r="AQ24" s="58">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0.31948881789137379</v>
       </c>
       <c r="AR24" s="58">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0.50251256281407031</v>
       </c>
       <c r="AS24" s="58">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0.22727272727272727</v>
       </c>
       <c r="AT24" s="30">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0.69444444444444442</v>
       </c>
       <c r="AU24" s="23"/>
     </row>
-    <row r="26" spans="1:58">
+    <row r="26" spans="1:59">
       <c r="G26" t="s">
         <v>170</v>
       </c>
@@ -4918,7 +5012,7 @@
         <v>0.22600000000000001</v>
       </c>
     </row>
-    <row r="27" spans="1:58">
+    <row r="27" spans="1:59">
       <c r="A27" t="s">
         <v>214</v>
       </c>
@@ -4930,27 +5024,27 @@
         <v>208</v>
       </c>
     </row>
-    <row r="28" spans="1:58">
+    <row r="28" spans="1:59">
       <c r="G28" t="s">
         <v>166</v>
       </c>
       <c r="AO28" s="68"/>
-      <c r="AP28" s="88" t="s">
+      <c r="AP28" s="89" t="s">
         <v>207</v>
       </c>
-      <c r="AQ28" s="88"/>
-      <c r="AR28" s="88"/>
-      <c r="AS28" s="88"/>
+      <c r="AQ28" s="89"/>
+      <c r="AR28" s="89"/>
+      <c r="AS28" s="89"/>
       <c r="AT28" s="72"/>
       <c r="AU28" s="68"/>
-      <c r="AV28" s="88" t="s">
+      <c r="AV28" s="89" t="s">
         <v>206</v>
       </c>
-      <c r="AW28" s="88"/>
-      <c r="AX28" s="88"/>
-      <c r="AY28" s="88"/>
-    </row>
-    <row r="29" spans="1:58" ht="30">
+      <c r="AW28" s="89"/>
+      <c r="AX28" s="89"/>
+      <c r="AY28" s="89"/>
+    </row>
+    <row r="29" spans="1:59" ht="30">
       <c r="G29" t="s">
         <v>171</v>
       </c>
@@ -4986,7 +5080,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="30" spans="1:58">
+    <row r="30" spans="1:59">
       <c r="G30" t="s">
         <v>172</v>
       </c>
@@ -5028,7 +5122,7 @@
         <v>0.14903129657228018</v>
       </c>
     </row>
-    <row r="31" spans="1:58">
+    <row r="31" spans="1:59">
       <c r="AO31" s="62" t="s">
         <v>200</v>
       </c>
@@ -5067,7 +5161,7 @@
         <v>4.4111160123511246E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:58">
+    <row r="32" spans="1:59">
       <c r="AO32" s="32" t="s">
         <v>162</v>
       </c>
@@ -5193,19 +5287,19 @@
     </row>
     <row r="37" spans="41:51" ht="31" customHeight="1">
       <c r="AO37" s="68"/>
-      <c r="AP37" s="88" t="s">
+      <c r="AP37" s="89" t="s">
         <v>204</v>
       </c>
-      <c r="AQ37" s="88"/>
-      <c r="AR37" s="88"/>
-      <c r="AS37" s="88"/>
+      <c r="AQ37" s="89"/>
+      <c r="AR37" s="89"/>
+      <c r="AS37" s="89"/>
       <c r="AU37" s="68"/>
-      <c r="AV37" s="88" t="s">
+      <c r="AV37" s="89" t="s">
         <v>205</v>
       </c>
-      <c r="AW37" s="88"/>
-      <c r="AX37" s="88"/>
-      <c r="AY37" s="88"/>
+      <c r="AW37" s="89"/>
+      <c r="AX37" s="89"/>
+      <c r="AY37" s="89"/>
     </row>
     <row r="38" spans="41:51">
       <c r="AO38" s="32" t="s">
@@ -5458,7 +5552,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="B1:AF50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="R3" sqref="R3"/>
     </sheetView>
   </sheetViews>
@@ -7984,31 +8078,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="15.5" thickBot="1">
-      <c r="A1" s="84" t="s">
+      <c r="A1" s="85" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="80" t="s">
+      <c r="B1" s="81" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="80" t="s">
+      <c r="C1" s="81" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="77" t="s">
+      <c r="D1" s="78" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="78"/>
-      <c r="F1" s="78"/>
-      <c r="G1" s="78"/>
-      <c r="H1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
+      <c r="G1" s="79"/>
+      <c r="H1" s="80"/>
     </row>
     <row r="2" spans="1:17" ht="42">
-      <c r="A2" s="85"/>
-      <c r="B2" s="87"/>
-      <c r="C2" s="87"/>
-      <c r="D2" s="80" t="s">
+      <c r="A2" s="86"/>
+      <c r="B2" s="88"/>
+      <c r="C2" s="88"/>
+      <c r="D2" s="81" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="80" t="s">
+      <c r="E2" s="81" t="s">
         <v>24</v>
       </c>
       <c r="F2" s="9" t="s">
@@ -8017,7 +8111,7 @@
       <c r="G2" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="H2" s="80" t="s">
+      <c r="H2" s="81" t="s">
         <v>29</v>
       </c>
       <c r="K2" s="17" t="s">
@@ -8031,18 +8125,18 @@
       <c r="Q2" s="18"/>
     </row>
     <row r="3" spans="1:17" ht="47" thickBot="1">
-      <c r="A3" s="86"/>
-      <c r="B3" s="81"/>
-      <c r="C3" s="81"/>
-      <c r="D3" s="81"/>
-      <c r="E3" s="81"/>
+      <c r="A3" s="87"/>
+      <c r="B3" s="82"/>
+      <c r="C3" s="82"/>
+      <c r="D3" s="82"/>
+      <c r="E3" s="82"/>
       <c r="F3" s="7" t="s">
         <v>26</v>
       </c>
       <c r="G3" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="H3" s="81"/>
+      <c r="H3" s="82"/>
       <c r="K3" s="18" t="s">
         <v>19</v>
       </c>

</xml_diff>